<commit_message>
Added User stories & Acceptance criteria to User_Stories.xlsx and added 10 User stories issues to User_Stories_ISsues.docx
</commit_message>
<xml_diff>
--- a/Requirement_Analysis/User_Stories.xlsx
+++ b/Requirement_Analysis/User_Stories.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SWCM\DemoBlaze_Project\Requirement_Analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5E036B-128C-44B3-9F45-0EA48AFD348B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="User Stories" sheetId="1" r:id="rId1"/>
+    <sheet name="Observations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +25,67 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>User Story #3:
+As a visitor, I want to browse the catalgoue of products so I can decide if I will make a purchase before registering</t>
+  </si>
+  <si>
+    <t>User Story #2:
+As a registered user, I want to see my purchase history so I can track my expenses with this vendor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no inherent value in registering </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no purchase history available </t>
+  </si>
+  <si>
+    <t>When checking out, any invalid input is accepted</t>
+  </si>
+  <si>
+    <t>When adding a product, It has to be added 1 by 1, a +- counter would be better here</t>
+  </si>
+  <si>
+    <t>Homepage Categories acts a filter within same url</t>
+  </si>
+  <si>
+    <t>No item sort option, Displayed items are not sorted in any way</t>
+  </si>
+  <si>
+    <t>Pressing next or previous after pressing a category merges all product log again</t>
+  </si>
+  <si>
+    <t>Cart is properly configured if you're logged in and refresh/log out-log in again/use a different browser/ use incognito and logging in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cart remembers your addition if you're logged out and add items, this should be reset on page refresh or session end. </t>
+  </si>
+  <si>
+    <t>User Story #1:
+As a buyer, I want to add products to my cart so that I can check out and pay for my goods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Openning "https://www.demoblaze.com/cart.html" from a different browser or incognito without logging in displays a gigantic cart, probably from all the unregistered users testing the website </t>
+  </si>
+  <si>
+    <t>Acceptance Criteria: 
+Given a person registered and logged in and already did a purchase, when they click on their "Welcome, USERNAME" button, then the user should be redirected to a profile page showing purchase history</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria: 
+Given a person a person wants to browse and shop, when they visit "https://www.demoblaze.com/index.html" , then they will see the exact same catalogue of items as the registered users without restrictions</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria: 
+Given a person on a product's page, When they press on a "Add to cart", then the product will be added with it's respective price to the user's cart -Accessible from header option- and are able to pay for their goods afterwards.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +115,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +402,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="94.5703125" customWidth="1"/>
+    <col min="2" max="2" width="91.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEE0EBE-ECF6-42F9-A62C-E224A3BF0EC1}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="169.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>